<commit_message>
feat(lab-5): fix formatting and some text
</commit_message>
<xml_diff>
--- a/lab-5/Таблица требований.xlsx
+++ b/lab-5/Таблица требований.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhXsEDPvMAyRvCD2m8p7MOqeriBWQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhVI4s5P73ML3E+7K/7wv1yT6+7ow=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Приоритет : 1- важно, 2-средняя важность, 3 - не важно</t>
   </si>
@@ -69,6 +69,9 @@
     <t>возможность назначения модератора</t>
   </si>
   <si>
+    <t>Не важно</t>
+  </si>
+  <si>
     <t>Модератор</t>
   </si>
   <si>
@@ -81,9 +84,6 @@
     <t>проверка задач на правильное оформление отсутствие нецензурного контента</t>
   </si>
   <si>
-    <t>Не важно</t>
-  </si>
-  <si>
     <t>Пользователь</t>
   </si>
   <si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>возможность регистрации</t>
-  </si>
-  <si>
-    <t>Не  важно</t>
   </si>
   <si>
     <t>возможность создания задания с последующей регистрацией</t>
@@ -127,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -143,13 +140,18 @@
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -306,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -333,67 +335,64 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +833,8 @@
       <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10">
-        <v>1.0</v>
+      <c r="E7" s="14">
+        <v>2.0</v>
       </c>
       <c r="F7" s="11">
         <v>2.0</v>
@@ -899,21 +898,21 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>10</v>
+      <c r="D9" s="17" t="s">
+        <v>17</v>
       </c>
-      <c r="E9" s="15">
-        <v>1.0</v>
+      <c r="E9" s="17">
+        <v>3.0</v>
       </c>
-      <c r="F9" s="16">
-        <v>1.0</v>
+      <c r="F9" s="18">
+        <v>3.0</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -937,17 +936,17 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="10">
         <v>3.0</v>
@@ -978,7 +977,7 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>12</v>
@@ -1014,15 +1013,15 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
-        <v>20</v>
+      <c r="A12" s="15"/>
+      <c r="B12" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E12" s="20">
         <v>1.0</v>
@@ -1098,8 +1097,8 @@
       <c r="C14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>25</v>
+      <c r="D14" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="E14" s="10">
         <v>2.0</v>
@@ -1131,9 +1130,9 @@
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="23" t="s">
@@ -1142,7 +1141,7 @@
       <c r="E15" s="23">
         <v>1.0</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="24">
         <v>1.0</v>
       </c>
       <c r="G15" s="4"/>
@@ -1167,22 +1166,22 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>27</v>
+      <c r="A16" s="25" t="s">
+        <v>26</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>18</v>
+      <c r="B16" s="26" t="s">
+        <v>19</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>2.0</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="27">
         <v>2.0</v>
       </c>
       <c r="G16" s="4"/>
@@ -1208,18 +1207,18 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="B17" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="10">
         <v>1.0</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="11">
         <v>1.0</v>
       </c>
       <c r="G17" s="4"/>
@@ -1245,10 +1244,10 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="B18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>30</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>10</v>
@@ -1282,9 +1281,9 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="B19" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="10" t="s">
@@ -1319,19 +1318,19 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="B20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="10">
-        <v>1.0</v>
+      <c r="E20" s="14">
+        <v>2.0</v>
       </c>
-      <c r="F20" s="11">
-        <v>1.0</v>
+      <c r="F20" s="28">
+        <v>2.0</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1355,21 +1354,21 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="19" t="s">
-        <v>33</v>
+      <c r="A21" s="15"/>
+      <c r="B21" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>34</v>
+      <c r="D21" s="20" t="s">
+        <v>33</v>
       </c>
-      <c r="E21" s="19">
-        <v>2.0</v>
+      <c r="E21" s="29">
+        <v>1.0</v>
       </c>
-      <c r="F21" s="31">
-        <v>2.0</v>
+      <c r="F21" s="30">
+        <v>1.0</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>

</xml_diff>